<commit_message>
Commiting exercies done in xls
</commit_message>
<xml_diff>
--- a/udacity/statistical_analysis/SD Social Networkers.xlsx
+++ b/udacity/statistical_analysis/SD Social Networkers.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="203" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="203" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Salaries of people with social network</t>
   </si>
@@ -36,6 +37,9 @@
   </si>
   <si>
     <t>standard deviation</t>
+  </si>
+  <si>
+    <t>Sample SD</t>
   </si>
 </sst>
 </file>
@@ -143,8 +147,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -332,4 +336,187 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">SUM(A3:A11) / 9</f>
+        <v>19.4444444444444</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">19.44444444 - A3</f>
+        <v>1.44444444</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">C3^2</f>
+        <v>2.08641974024692</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">SUM(D3:D11)/9</f>
+        <v>6.02469135802469</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">SQRT(E3)</f>
+        <v>2.45452467048606</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">19.44444444 - A4</f>
+        <v>-0.555555559999998</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">C4^2</f>
+        <v>0.308641980246912</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">19.44444444 - A5</f>
+        <v>-3.55555556</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">C5^2</f>
+        <v>12.6419753402469</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">19.44444444 - A6</f>
+        <v>1.44444444</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">C6^2</f>
+        <v>2.08641974024692</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">19.44444444 - A7</f>
+        <v>-2.55555556</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">C7^2</f>
+        <v>6.53086422024691</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">19.44444444 - A8</f>
+        <v>-1.55555556</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">C8^2</f>
+        <v>2.41975310024691</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">19.44444444 - A9</f>
+        <v>2.44444444</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">C9^2</f>
+        <v>5.97530862024692</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">19.44444444 - A10</f>
+        <v>-1.55555556</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">C10^2</f>
+        <v>2.41975310024691</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">19.44444444 - A11</f>
+        <v>4.44444444</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">C11^2</f>
+        <v>19.7530863802469</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>